<commit_message>
New example: Contractual Setting
</commit_message>
<xml_diff>
--- a/Session 04/01-exercises/data/s4.xlsx
+++ b/Session 04/01-exercises/data/s4.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josepcurto/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josepcurto/Documents/Work/3. Teaching/IE/Business School/Customer Analytics/01-Sessions/S4/01-exercises/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35601BB6-AABF-9141-9E83-22CB75DC8DA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="520" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="980" yWindow="520" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ex1" sheetId="1" r:id="rId1"/>
-    <sheet name="Ex2" sheetId="2" r:id="rId2"/>
+    <sheet name="ex1" sheetId="1" r:id="rId1"/>
+    <sheet name="ex2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,25 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>CustomerName</t>
   </si>
@@ -61,12 +44,21 @@
   </si>
   <si>
     <t>Laura</t>
+  </si>
+  <si>
+    <t>activeCust</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>lostCust</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -108,6 +100,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -375,10 +370,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -386,18 +381,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>42005</v>
@@ -408,7 +403,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>42109</v>
@@ -419,7 +414,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>42170</v>
@@ -430,7 +425,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>42095</v>
@@ -441,7 +436,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>42170</v>
@@ -452,7 +447,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
         <v>42185</v>
@@ -467,173 +462,101 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40196617-EC00-FC42-A422-8BB411A564A4}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>869</v>
       </c>
       <c r="C2">
-        <v>375</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>0.01</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>165</v>
+        <v>743</v>
       </c>
       <c r="C3">
-        <v>375</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>0.01</v>
-      </c>
-      <c r="F3">
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>150</v>
+        <v>653</v>
       </c>
       <c r="C4">
-        <v>375</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>0.01</v>
-      </c>
-      <c r="F4">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>176</v>
+        <v>593</v>
       </c>
       <c r="C5">
-        <v>375</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>0.01</v>
-      </c>
-      <c r="F5">
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>178</v>
+        <v>551</v>
       </c>
       <c r="C6">
-        <v>375</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>0.01</v>
-      </c>
-      <c r="F6">
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>150</v>
+        <v>517</v>
       </c>
       <c r="C7">
-        <v>375</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>0.01</v>
-      </c>
-      <c r="F7">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>135</v>
+        <v>491</v>
       </c>
       <c r="C8">
-        <v>375</v>
-      </c>
-      <c r="D8">
-        <v>20</v>
-      </c>
-      <c r="E8">
-        <v>0.01</v>
-      </c>
-      <c r="F8">
-        <v>0.9</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>